<commit_message>
Adds create_excel function and improves traveler template.
</commit_message>
<xml_diff>
--- a/TravelerTemplate.xlsx
+++ b/TravelerTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cam Nguyen\Documents\GitHub\XometryParsePDF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747500A4-5D81-49F6-A291-9304AA5745E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F8FDF5-F52C-4A31-A50A-BE4D05172A46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31140" yWindow="4095" windowWidth="27930" windowHeight="15885" xr2:uid="{23A2CD55-8510-467F-B1BF-73F4125FC08A}"/>
+    <workbookView xWindow="-29460" yWindow="4005" windowWidth="27930" windowHeight="15885" xr2:uid="{23A2CD55-8510-467F-B1BF-73F4125FC08A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Purchase Order</t>
   </si>
@@ -64,13 +64,16 @@
   </si>
   <si>
     <t>Inspection Requirements</t>
+  </si>
+  <si>
+    <t>NOTES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,14 +83,22 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
+      <sz val="32"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -108,7 +119,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -177,17 +188,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -207,14 +273,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -535,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E2119EE-1AD4-42E6-A8C1-991A57AD1238}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:C12"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="54" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -549,26 +621,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" ht="21.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" ht="138.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,12 +651,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="72" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="21.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -595,12 +667,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="72" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" ht="21.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -611,30 +683,113 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="72" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" ht="21.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:3" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-    </row>
-    <row r="13" spans="1:3" ht="54" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="1:3" ht="72" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+    </row>
+    <row r="14" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+    </row>
+    <row r="15" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+    </row>
+    <row r="18" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+    </row>
+    <row r="19" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+    </row>
+    <row r="20" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+    </row>
+    <row r="21" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+    </row>
+    <row r="22" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+    </row>
+    <row r="23" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+    </row>
+    <row r="24" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+    </row>
+    <row r="25" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+    </row>
+    <row r="27" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="A14:C26"/>
     <mergeCell ref="A2:C4"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>